<commit_message>
minor edits to pages
</commit_message>
<xml_diff>
--- a/docs/q.xlsx
+++ b/docs/q.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2199" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2199" uniqueCount="387">
   <si>
     <t>Path</t>
   </si>
@@ -364,7 +364,7 @@
     <t>Can be a urn:uuid: or a urn:oid:, but real http: addresses are preferred.  Multiple instances may share the same url if they have a distinct version.</t>
   </si>
   <si>
-    <t>…  This is the id that will be used to link a QuestionnaireResponse to the Questionnaire the response is for.</t>
+    <t>This is the id that will be used to link a QuestionnaireResponse to the Questionnaire .</t>
   </si>
   <si>
     <t>New Element in R3</t>
@@ -698,9 +698,6 @@
   </si>
   <si>
     <t>May be a web site, an email address, a telephone number, etc.</t>
-  </si>
-  <si>
-    <t>Questionnaire.telecom</t>
   </si>
   <si>
     <t>.participation[typeCode=CALLBCK].role</t>
@@ -1025,9 +1022,6 @@
 </t>
   </si>
   <si>
-    <t>Questionnaire.item.enableWhen.operator</t>
-  </si>
-  <si>
     <t>Questionnaire.item.enableWhen.answer[x]</t>
   </si>
   <si>
@@ -1216,9 +1210,6 @@
   <si>
     <t xml:space="preserve">que-8
 </t>
-  </si>
-  <si>
-    <t>Questionnaire.item.initial.value[x]</t>
   </si>
   <si>
     <t>Questionnaire.item.item</t>
@@ -1436,7 +1427,7 @@
     <col min="33" max="33" width="9.890625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="34" max="34" width="12.71875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="36" max="36" width="40.546875" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="33.5" customWidth="true" bestFit="true"/>
     <col min="37" max="37" width="66.61328125" customWidth="true" bestFit="true"/>
     <col min="38" max="38" width="126.8984375" customWidth="true" bestFit="true"/>
     <col min="39" max="39" width="25.74609375" customWidth="true" bestFit="true"/>
@@ -2618,7 +2609,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" hidden="true">
+    <row r="11">
       <c r="A11" t="s" s="2">
         <v>107</v>
       </c>
@@ -2628,13 +2619,13 @@
       </c>
       <c r="D11" s="2"/>
       <c r="E11" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="F11" t="s" s="2">
         <v>52</v>
       </c>
       <c r="G11" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H11" t="s" s="2">
         <v>45</v>
@@ -2838,10 +2829,10 @@
         <v>45</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="AK12" t="s" s="2">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="AL12" t="s" s="2">
         <v>121</v>
@@ -2856,7 +2847,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" hidden="true">
+    <row r="13">
       <c r="A13" t="s" s="2">
         <v>123</v>
       </c>
@@ -2872,7 +2863,7 @@
         <v>52</v>
       </c>
       <c r="G13" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H13" t="s" s="2">
         <v>45</v>
@@ -3074,10 +3065,10 @@
         <v>45</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>130</v>
+        <v>45</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="AL14" t="s" s="2">
         <v>95</v>
@@ -3092,7 +3083,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" hidden="true">
+    <row r="15">
       <c r="A15" t="s" s="2">
         <v>135</v>
       </c>
@@ -3102,13 +3093,13 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="F15" t="s" s="2">
         <v>52</v>
       </c>
       <c r="G15" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H15" t="s" s="2">
         <v>45</v>
@@ -3209,7 +3200,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" hidden="true">
+    <row r="16">
       <c r="A16" t="s" s="2">
         <v>140</v>
       </c>
@@ -3225,7 +3216,7 @@
         <v>52</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H16" t="s" s="2">
         <v>53</v>
@@ -3427,10 +3418,10 @@
         <v>45</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>149</v>
+        <v>45</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="AL17" t="s" s="2">
         <v>95</v>
@@ -3544,10 +3535,10 @@
         <v>45</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>156</v>
+        <v>45</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>156</v>
+        <v>45</v>
       </c>
       <c r="AL18" t="s" s="2">
         <v>162</v>
@@ -3663,10 +3654,10 @@
         <v>45</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>164</v>
+        <v>45</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>164</v>
+        <v>45</v>
       </c>
       <c r="AL19" t="s" s="2">
         <v>169</v>
@@ -3681,7 +3672,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" hidden="true">
+    <row r="20">
       <c r="A20" t="s" s="2">
         <v>171</v>
       </c>
@@ -3697,7 +3688,7 @@
         <v>52</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H20" t="s" s="2">
         <v>45</v>
@@ -3897,10 +3888,10 @@
         <v>45</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>177</v>
+        <v>45</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="AL21" t="s" s="2">
         <v>181</v>
@@ -4014,10 +4005,10 @@
         <v>45</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>183</v>
+        <v>45</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="AL22" t="s" s="2">
         <v>188</v>
@@ -4133,10 +4124,10 @@
         <v>45</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>189</v>
+        <v>45</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="AL23" t="s" s="2">
         <v>194</v>
@@ -4252,10 +4243,10 @@
         <v>45</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>195</v>
+        <v>45</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="AL24" t="s" s="2">
         <v>128</v>
@@ -4371,10 +4362,10 @@
         <v>45</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>201</v>
+        <v>45</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="AL25" t="s" s="2">
         <v>128</v>
@@ -4488,10 +4479,10 @@
         <v>45</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>207</v>
+        <v>45</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="AL26" t="s" s="2">
         <v>128</v>
@@ -4605,13 +4596,13 @@
         <v>45</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>214</v>
+        <v>45</v>
       </c>
       <c r="AK27" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL27" t="s" s="2">
         <v>219</v>
-      </c>
-      <c r="AL27" t="s" s="2">
-        <v>220</v>
       </c>
       <c r="AM27" t="s" s="2">
         <v>45</v>
@@ -4625,11 +4616,11 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" t="s" s="2">
@@ -4651,14 +4642,14 @@
         <v>172</v>
       </c>
       <c r="K28" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="L28" t="s" s="2">
         <v>223</v>
-      </c>
-      <c r="L28" t="s" s="2">
-        <v>224</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" t="s" s="2">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O28" t="s" s="2">
         <v>45</v>
@@ -4707,7 +4698,7 @@
         <v>45</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>43</v>
@@ -4722,10 +4713,10 @@
         <v>45</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>221</v>
+        <v>45</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="AL28" t="s" s="2">
         <v>128</v>
@@ -4742,7 +4733,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4765,17 +4756,17 @@
         <v>53</v>
       </c>
       <c r="J29" t="s" s="2">
+        <v>226</v>
+      </c>
+      <c r="K29" t="s" s="2">
         <v>227</v>
       </c>
-      <c r="K29" t="s" s="2">
+      <c r="L29" t="s" s="2">
         <v>228</v>
-      </c>
-      <c r="L29" t="s" s="2">
-        <v>229</v>
       </c>
       <c r="M29" s="2"/>
       <c r="N29" t="s" s="2">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="O29" t="s" s="2">
         <v>45</v>
@@ -4800,14 +4791,14 @@
         <v>45</v>
       </c>
       <c r="W29" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="X29" t="s" s="2">
         <v>231</v>
       </c>
-      <c r="X29" t="s" s="2">
+      <c r="Y29" t="s" s="2">
         <v>232</v>
       </c>
-      <c r="Y29" t="s" s="2">
-        <v>233</v>
-      </c>
       <c r="Z29" t="s" s="2">
         <v>45</v>
       </c>
@@ -4824,7 +4815,7 @@
         <v>45</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>43</v>
@@ -4839,13 +4830,13 @@
         <v>45</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>226</v>
+        <v>45</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AM29" t="s" s="2">
         <v>45</v>
@@ -4859,7 +4850,7 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4885,13 +4876,13 @@
         <v>71</v>
       </c>
       <c r="K30" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="L30" t="s" s="2">
         <v>236</v>
       </c>
-      <c r="L30" t="s" s="2">
+      <c r="M30" t="s" s="2">
         <v>237</v>
-      </c>
-      <c r="M30" t="s" s="2">
-        <v>238</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
@@ -4920,11 +4911,11 @@
         <v>144</v>
       </c>
       <c r="X30" t="s" s="2">
+        <v>238</v>
+      </c>
+      <c r="Y30" t="s" s="2">
         <v>239</v>
       </c>
-      <c r="Y30" t="s" s="2">
-        <v>240</v>
-      </c>
       <c r="Z30" t="s" s="2">
         <v>45</v>
       </c>
@@ -4941,7 +4932,7 @@
         <v>45</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
@@ -4956,27 +4947,27 @@
         <v>45</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>235</v>
+        <v>45</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>235</v>
+        <v>45</v>
       </c>
       <c r="AL30" t="s" s="2">
+        <v>240</v>
+      </c>
+      <c r="AM30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AN30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO30" t="s" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="2">
         <v>241</v>
-      </c>
-      <c r="AM30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AN30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO30" t="s" s="2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="31" hidden="true">
-      <c r="A31" t="s" s="2">
-        <v>242</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4990,7 +4981,7 @@
         <v>44</v>
       </c>
       <c r="G31" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H31" t="s" s="2">
         <v>45</v>
@@ -4999,16 +4990,16 @@
         <v>45</v>
       </c>
       <c r="J31" t="s" s="2">
+        <v>242</v>
+      </c>
+      <c r="K31" t="s" s="2">
         <v>243</v>
       </c>
-      <c r="K31" t="s" s="2">
+      <c r="L31" t="s" s="2">
         <v>244</v>
       </c>
-      <c r="L31" t="s" s="2">
+      <c r="M31" t="s" s="2">
         <v>245</v>
-      </c>
-      <c r="M31" t="s" s="2">
-        <v>246</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
@@ -5058,7 +5049,7 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
@@ -5067,19 +5058,19 @@
         <v>44</v>
       </c>
       <c r="AH31" t="s" s="2">
+        <v>246</v>
+      </c>
+      <c r="AI31" t="s" s="2">
         <v>247</v>
       </c>
-      <c r="AI31" t="s" s="2">
+      <c r="AJ31" t="s" s="2">
+        <v>241</v>
+      </c>
+      <c r="AK31" t="s" s="2">
         <v>248</v>
       </c>
-      <c r="AJ31" t="s" s="2">
-        <v>242</v>
-      </c>
-      <c r="AK31" t="s" s="2">
+      <c r="AL31" t="s" s="2">
         <v>249</v>
-      </c>
-      <c r="AL31" t="s" s="2">
-        <v>250</v>
       </c>
       <c r="AM31" t="s" s="2">
         <v>45</v>
@@ -5093,7 +5084,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5119,10 +5110,10 @@
         <v>124</v>
       </c>
       <c r="K32" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="L32" t="s" s="2">
         <v>252</v>
-      </c>
-      <c r="L32" t="s" s="2">
-        <v>253</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -5173,28 +5164,28 @@
         <v>45</v>
       </c>
       <c r="AE32" t="s" s="2">
+        <v>253</v>
+      </c>
+      <c r="AF32" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG32" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL32" t="s" s="2">
         <v>254</v>
-      </c>
-      <c r="AF32" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG32" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL32" t="s" s="2">
-        <v>255</v>
       </c>
       <c r="AM32" t="s" s="2">
         <v>45</v>
@@ -5208,7 +5199,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5237,7 +5228,7 @@
         <v>99</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="M33" t="s" s="2">
         <v>101</v>
@@ -5290,7 +5281,7 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
@@ -5311,7 +5302,7 @@
         <v>45</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AM33" t="s" s="2">
         <v>45</v>
@@ -5325,11 +5316,11 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
@@ -5354,7 +5345,7 @@
         <v>104</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="M34" t="s" s="2">
         <v>101</v>
@@ -5407,7 +5398,7 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5440,9 +5431,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" hidden="true">
+    <row r="35">
       <c r="A35" t="s" s="2">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5456,7 +5447,7 @@
         <v>52</v>
       </c>
       <c r="G35" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H35" t="s" s="2">
         <v>45</v>
@@ -5468,16 +5459,16 @@
         <v>124</v>
       </c>
       <c r="K35" t="s" s="2">
+        <v>263</v>
+      </c>
+      <c r="L35" t="s" s="2">
         <v>264</v>
       </c>
-      <c r="L35" t="s" s="2">
+      <c r="M35" t="s" s="2">
         <v>265</v>
       </c>
-      <c r="M35" t="s" s="2">
+      <c r="N35" t="s" s="2">
         <v>266</v>
-      </c>
-      <c r="N35" t="s" s="2">
-        <v>267</v>
       </c>
       <c r="O35" t="s" s="2">
         <v>45</v>
@@ -5526,7 +5517,7 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>52</v>
@@ -5541,13 +5532,13 @@
         <v>45</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AK35" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="AL35" t="s" s="2">
         <v>268</v>
-      </c>
-      <c r="AL35" t="s" s="2">
-        <v>269</v>
       </c>
       <c r="AM35" t="s" s="2">
         <v>45</v>
@@ -5561,7 +5552,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5587,16 +5578,16 @@
         <v>65</v>
       </c>
       <c r="K36" t="s" s="2">
+        <v>270</v>
+      </c>
+      <c r="L36" t="s" s="2">
         <v>271</v>
       </c>
-      <c r="L36" t="s" s="2">
+      <c r="M36" t="s" s="2">
         <v>272</v>
       </c>
-      <c r="M36" t="s" s="2">
+      <c r="N36" t="s" s="2">
         <v>273</v>
-      </c>
-      <c r="N36" t="s" s="2">
-        <v>274</v>
       </c>
       <c r="O36" t="s" s="2">
         <v>45</v>
@@ -5645,7 +5636,7 @@
         <v>45</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>43</v>
@@ -5660,27 +5651,27 @@
         <v>45</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>270</v>
+        <v>45</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="AL36" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="AM36" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AN36" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO36" t="s" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="2">
         <v>275</v>
-      </c>
-      <c r="AM36" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AN36" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO36" t="s" s="2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="37" hidden="true">
-      <c r="A37" t="s" s="2">
-        <v>276</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5694,7 +5685,7 @@
         <v>44</v>
       </c>
       <c r="G37" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H37" t="s" s="2">
         <v>45</v>
@@ -5703,19 +5694,19 @@
         <v>53</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K37" t="s" s="2">
+        <v>276</v>
+      </c>
+      <c r="L37" t="s" s="2">
         <v>277</v>
       </c>
-      <c r="L37" t="s" s="2">
+      <c r="M37" t="s" s="2">
         <v>278</v>
       </c>
-      <c r="M37" t="s" s="2">
+      <c r="N37" t="s" s="2">
         <v>279</v>
-      </c>
-      <c r="N37" t="s" s="2">
-        <v>280</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>45</v>
@@ -5740,14 +5731,14 @@
         <v>45</v>
       </c>
       <c r="W37" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="X37" t="s" s="2">
         <v>231</v>
       </c>
-      <c r="X37" t="s" s="2">
+      <c r="Y37" t="s" s="2">
         <v>232</v>
       </c>
-      <c r="Y37" t="s" s="2">
-        <v>233</v>
-      </c>
       <c r="Z37" t="s" s="2">
         <v>45</v>
       </c>
@@ -5764,7 +5755,7 @@
         <v>45</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
@@ -5773,37 +5764,37 @@
         <v>44</v>
       </c>
       <c r="AH37" t="s" s="2">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AI37" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AK37" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="AL37" t="s" s="2">
+        <v>233</v>
+      </c>
+      <c r="AM37" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AN37" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO37" t="s" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="2">
         <v>281</v>
-      </c>
-      <c r="AL37" t="s" s="2">
-        <v>234</v>
-      </c>
-      <c r="AM37" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AN37" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO37" t="s" s="2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="38" hidden="true">
-      <c r="A38" t="s" s="2">
-        <v>282</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" t="s" s="2">
@@ -5813,7 +5804,7 @@
         <v>52</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H38" t="s" s="2">
         <v>45</v>
@@ -5825,16 +5816,16 @@
         <v>124</v>
       </c>
       <c r="K38" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="L38" t="s" s="2">
         <v>284</v>
       </c>
-      <c r="L38" t="s" s="2">
+      <c r="M38" t="s" s="2">
         <v>285</v>
       </c>
-      <c r="M38" t="s" s="2">
+      <c r="N38" t="s" s="2">
         <v>286</v>
-      </c>
-      <c r="N38" t="s" s="2">
-        <v>287</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>45</v>
@@ -5883,7 +5874,7 @@
         <v>45</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>43</v>
@@ -5898,27 +5889,27 @@
         <v>45</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AK38" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="AL38" t="s" s="2">
         <v>288</v>
       </c>
-      <c r="AL38" t="s" s="2">
+      <c r="AM38" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AN38" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO38" t="s" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="2">
         <v>289</v>
-      </c>
-      <c r="AM38" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AN38" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO38" t="s" s="2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="39" hidden="true">
-      <c r="A39" t="s" s="2">
-        <v>290</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5932,7 +5923,7 @@
         <v>52</v>
       </c>
       <c r="G39" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H39" t="s" s="2">
         <v>45</v>
@@ -5944,10 +5935,10 @@
         <v>124</v>
       </c>
       <c r="K39" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="L39" t="s" s="2">
         <v>291</v>
-      </c>
-      <c r="L39" t="s" s="2">
-        <v>292</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -5998,7 +5989,7 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
@@ -6013,10 +6004,10 @@
         <v>45</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AL39" t="s" s="2">
         <v>176</v>
@@ -6031,9 +6022,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" hidden="true">
+    <row r="40">
       <c r="A40" t="s" s="2">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6047,7 +6038,7 @@
         <v>52</v>
       </c>
       <c r="G40" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H40" t="s" s="2">
         <v>45</v>
@@ -6059,16 +6050,16 @@
         <v>71</v>
       </c>
       <c r="K40" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="L40" t="s" s="2">
         <v>295</v>
       </c>
-      <c r="L40" t="s" s="2">
+      <c r="M40" t="s" s="2">
         <v>296</v>
       </c>
-      <c r="M40" t="s" s="2">
+      <c r="N40" t="s" s="2">
         <v>297</v>
-      </c>
-      <c r="N40" t="s" s="2">
-        <v>298</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>45</v>
@@ -6096,49 +6087,49 @@
         <v>144</v>
       </c>
       <c r="X40" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="Y40" t="s" s="2">
         <v>299</v>
       </c>
-      <c r="Y40" t="s" s="2">
+      <c r="Z40" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA40" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB40" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC40" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD40" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE40" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="AF40" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AG40" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH40" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI40" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ40" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="AK40" t="s" s="2">
         <v>300</v>
       </c>
-      <c r="Z40" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA40" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB40" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC40" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD40" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE40" t="s" s="2">
-        <v>294</v>
-      </c>
-      <c r="AF40" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AG40" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH40" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI40" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ40" t="s" s="2">
-        <v>294</v>
-      </c>
-      <c r="AK40" t="s" s="2">
+      <c r="AL40" t="s" s="2">
         <v>301</v>
-      </c>
-      <c r="AL40" t="s" s="2">
-        <v>302</v>
       </c>
       <c r="AM40" t="s" s="2">
         <v>45</v>
@@ -6152,7 +6143,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6175,19 +6166,19 @@
         <v>53</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K41" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="L41" t="s" s="2">
         <v>304</v>
       </c>
-      <c r="L41" t="s" s="2">
+      <c r="M41" t="s" s="2">
         <v>305</v>
       </c>
-      <c r="M41" t="s" s="2">
+      <c r="N41" t="s" s="2">
         <v>306</v>
-      </c>
-      <c r="N41" t="s" s="2">
-        <v>307</v>
       </c>
       <c r="O41" t="s" s="2">
         <v>45</v>
@@ -6236,7 +6227,7 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
@@ -6248,16 +6239,16 @@
         <v>45</v>
       </c>
       <c r="AI41" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>303</v>
+        <v>45</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AM41" t="s" s="2">
         <v>45</v>
@@ -6271,7 +6262,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6297,10 +6288,10 @@
         <v>124</v>
       </c>
       <c r="K42" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="L42" t="s" s="2">
         <v>252</v>
-      </c>
-      <c r="L42" t="s" s="2">
-        <v>253</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -6351,28 +6342,28 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
+        <v>253</v>
+      </c>
+      <c r="AF42" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG42" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH42" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI42" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ42" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK42" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL42" t="s" s="2">
         <v>254</v>
-      </c>
-      <c r="AF42" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG42" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH42" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI42" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ42" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK42" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL42" t="s" s="2">
-        <v>255</v>
       </c>
       <c r="AM42" t="s" s="2">
         <v>45</v>
@@ -6386,7 +6377,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6415,7 +6406,7 @@
         <v>99</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="M43" t="s" s="2">
         <v>101</v>
@@ -6468,7 +6459,7 @@
         <v>45</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
@@ -6489,7 +6480,7 @@
         <v>45</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AM43" t="s" s="2">
         <v>45</v>
@@ -6503,11 +6494,11 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" t="s" s="2">
@@ -6532,7 +6523,7 @@
         <v>104</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="M44" t="s" s="2">
         <v>101</v>
@@ -6585,7 +6576,7 @@
         <v>45</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
@@ -6620,7 +6611,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6646,13 +6637,13 @@
         <v>124</v>
       </c>
       <c r="K45" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="L45" t="s" s="2">
         <v>313</v>
       </c>
-      <c r="L45" t="s" s="2">
+      <c r="M45" t="s" s="2">
         <v>314</v>
-      </c>
-      <c r="M45" t="s" s="2">
-        <v>315</v>
       </c>
       <c r="N45" s="2"/>
       <c r="O45" t="s" s="2">
@@ -6702,7 +6693,7 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>52</v>
@@ -6717,13 +6708,13 @@
         <v>45</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>312</v>
+        <v>45</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AM45" t="s" s="2">
         <v>45</v>
@@ -6737,7 +6728,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6763,13 +6754,13 @@
         <v>150</v>
       </c>
       <c r="K46" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="L46" t="s" s="2">
         <v>317</v>
       </c>
-      <c r="L46" t="s" s="2">
+      <c r="M46" t="s" s="2">
         <v>318</v>
-      </c>
-      <c r="M46" t="s" s="2">
-        <v>319</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
@@ -6819,7 +6810,7 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
@@ -6828,19 +6819,19 @@
         <v>52</v>
       </c>
       <c r="AH46" t="s" s="2">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AI46" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>321</v>
+        <v>45</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AM46" t="s" s="2">
         <v>45</v>
@@ -6854,7 +6845,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6877,16 +6868,16 @@
         <v>45</v>
       </c>
       <c r="J47" t="s" s="2">
+        <v>321</v>
+      </c>
+      <c r="K47" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="L47" t="s" s="2">
         <v>323</v>
       </c>
-      <c r="K47" t="s" s="2">
+      <c r="M47" t="s" s="2">
         <v>324</v>
-      </c>
-      <c r="L47" t="s" s="2">
-        <v>325</v>
-      </c>
-      <c r="M47" t="s" s="2">
-        <v>326</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" t="s" s="2">
@@ -6912,66 +6903,66 @@
         <v>45</v>
       </c>
       <c r="W47" t="s" s="2">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="X47" t="s" s="2">
+        <v>325</v>
+      </c>
+      <c r="Y47" t="s" s="2">
+        <v>326</v>
+      </c>
+      <c r="Z47" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA47" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB47" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC47" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD47" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE47" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="AF47" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG47" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH47" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="AI47" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ47" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK47" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL47" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="AM47" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AN47" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO47" t="s" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="2">
         <v>327</v>
-      </c>
-      <c r="Y47" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="Z47" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA47" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB47" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC47" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD47" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE47" t="s" s="2">
-        <v>322</v>
-      </c>
-      <c r="AF47" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG47" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH47" t="s" s="2">
-        <v>320</v>
-      </c>
-      <c r="AI47" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ47" t="s" s="2">
-        <v>322</v>
-      </c>
-      <c r="AK47" t="s" s="2">
-        <v>112</v>
-      </c>
-      <c r="AL47" t="s" s="2">
-        <v>302</v>
-      </c>
-      <c r="AM47" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AN47" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO47" t="s" s="2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" hidden="true">
-      <c r="A48" t="s" s="2">
-        <v>329</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -6985,7 +6976,7 @@
         <v>52</v>
       </c>
       <c r="G48" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H48" t="s" s="2">
         <v>45</v>
@@ -6997,17 +6988,17 @@
         <v>150</v>
       </c>
       <c r="K48" t="s" s="2">
+        <v>328</v>
+      </c>
+      <c r="L48" t="s" s="2">
+        <v>329</v>
+      </c>
+      <c r="M48" t="s" s="2">
         <v>330</v>
-      </c>
-      <c r="L48" t="s" s="2">
-        <v>331</v>
-      </c>
-      <c r="M48" t="s" s="2">
-        <v>332</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="P48" s="2"/>
       <c r="Q48" t="s" s="2">
@@ -7053,7 +7044,7 @@
         <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>43</v>
@@ -7062,33 +7053,33 @@
         <v>52</v>
       </c>
       <c r="AH48" t="s" s="2">
+        <v>332</v>
+      </c>
+      <c r="AI48" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ48" t="s" s="2">
+        <v>327</v>
+      </c>
+      <c r="AK48" t="s" s="2">
+        <v>333</v>
+      </c>
+      <c r="AL48" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="AM48" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AN48" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO48" t="s" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="2">
         <v>334</v>
-      </c>
-      <c r="AI48" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ48" t="s" s="2">
-        <v>329</v>
-      </c>
-      <c r="AK48" t="s" s="2">
-        <v>335</v>
-      </c>
-      <c r="AL48" t="s" s="2">
-        <v>302</v>
-      </c>
-      <c r="AM48" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AN48" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO48" t="s" s="2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="49" hidden="true">
-      <c r="A49" t="s" s="2">
-        <v>336</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7102,7 +7093,7 @@
         <v>52</v>
       </c>
       <c r="G49" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H49" t="s" s="2">
         <v>45</v>
@@ -7114,19 +7105,19 @@
         <v>150</v>
       </c>
       <c r="K49" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="L49" t="s" s="2">
+        <v>336</v>
+      </c>
+      <c r="M49" t="s" s="2">
         <v>337</v>
       </c>
-      <c r="L49" t="s" s="2">
+      <c r="N49" t="s" s="2">
         <v>338</v>
       </c>
-      <c r="M49" t="s" s="2">
-        <v>339</v>
-      </c>
-      <c r="N49" t="s" s="2">
-        <v>340</v>
-      </c>
       <c r="O49" t="s" s="2">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="P49" s="2"/>
       <c r="Q49" t="s" s="2">
@@ -7172,7 +7163,7 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>43</v>
@@ -7181,19 +7172,19 @@
         <v>52</v>
       </c>
       <c r="AH49" t="s" s="2">
+        <v>332</v>
+      </c>
+      <c r="AI49" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ49" t="s" s="2">
         <v>334</v>
       </c>
-      <c r="AI49" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ49" t="s" s="2">
-        <v>336</v>
-      </c>
       <c r="AK49" t="s" s="2">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AM49" t="s" s="2">
         <v>45</v>
@@ -7207,7 +7198,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7233,16 +7224,16 @@
         <v>150</v>
       </c>
       <c r="K50" t="s" s="2">
+        <v>341</v>
+      </c>
+      <c r="L50" t="s" s="2">
+        <v>342</v>
+      </c>
+      <c r="M50" t="s" s="2">
         <v>343</v>
       </c>
-      <c r="L50" t="s" s="2">
+      <c r="N50" t="s" s="2">
         <v>344</v>
-      </c>
-      <c r="M50" t="s" s="2">
-        <v>345</v>
-      </c>
-      <c r="N50" t="s" s="2">
-        <v>346</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>45</v>
@@ -7291,7 +7282,7 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>43</v>
@@ -7300,19 +7291,19 @@
         <v>52</v>
       </c>
       <c r="AH50" t="s" s="2">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="AI50" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>342</v>
+        <v>45</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AM50" t="s" s="2">
         <v>45</v>
@@ -7326,7 +7317,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7349,16 +7340,16 @@
         <v>45</v>
       </c>
       <c r="J51" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="K51" t="s" s="2">
+        <v>348</v>
+      </c>
+      <c r="L51" t="s" s="2">
         <v>349</v>
       </c>
-      <c r="K51" t="s" s="2">
+      <c r="M51" t="s" s="2">
         <v>350</v>
-      </c>
-      <c r="L51" t="s" s="2">
-        <v>351</v>
-      </c>
-      <c r="M51" t="s" s="2">
-        <v>352</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" t="s" s="2">
@@ -7408,7 +7399,7 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>43</v>
@@ -7417,19 +7408,19 @@
         <v>52</v>
       </c>
       <c r="AH51" t="s" s="2">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="AI51" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>348</v>
+        <v>45</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AM51" t="s" s="2">
         <v>45</v>
@@ -7441,9 +7432,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="52" hidden="true">
+    <row r="52">
       <c r="A52" t="s" s="2">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7457,7 +7448,7 @@
         <v>52</v>
       </c>
       <c r="G52" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H52" t="s" s="2">
         <v>45</v>
@@ -7466,16 +7457,16 @@
         <v>45</v>
       </c>
       <c r="J52" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="K52" t="s" s="2">
+        <v>354</v>
+      </c>
+      <c r="L52" t="s" s="2">
         <v>355</v>
       </c>
-      <c r="K52" t="s" s="2">
+      <c r="M52" t="s" s="2">
         <v>356</v>
-      </c>
-      <c r="L52" t="s" s="2">
-        <v>357</v>
-      </c>
-      <c r="M52" t="s" s="2">
-        <v>358</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" t="s" s="2">
@@ -7525,7 +7516,7 @@
         <v>45</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>43</v>
@@ -7534,33 +7525,33 @@
         <v>52</v>
       </c>
       <c r="AH52" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="AI52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ52" t="s" s="2">
+        <v>352</v>
+      </c>
+      <c r="AK52" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="AL52" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="AM52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AN52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO52" t="s" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="2">
         <v>359</v>
-      </c>
-      <c r="AI52" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ52" t="s" s="2">
-        <v>354</v>
-      </c>
-      <c r="AK52" t="s" s="2">
-        <v>360</v>
-      </c>
-      <c r="AL52" t="s" s="2">
-        <v>302</v>
-      </c>
-      <c r="AM52" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AN52" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO52" t="s" s="2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="53" hidden="true">
-      <c r="A53" t="s" s="2">
-        <v>361</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7574,7 +7565,7 @@
         <v>44</v>
       </c>
       <c r="G53" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H53" t="s" s="2">
         <v>45</v>
@@ -7583,16 +7574,16 @@
         <v>45</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K53" t="s" s="2">
+        <v>360</v>
+      </c>
+      <c r="L53" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="M53" t="s" s="2">
         <v>362</v>
-      </c>
-      <c r="L53" t="s" s="2">
-        <v>363</v>
-      </c>
-      <c r="M53" t="s" s="2">
-        <v>364</v>
       </c>
       <c r="N53" s="2"/>
       <c r="O53" t="s" s="2">
@@ -7642,7 +7633,7 @@
         <v>45</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>43</v>
@@ -7651,19 +7642,19 @@
         <v>44</v>
       </c>
       <c r="AH53" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="AI53" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="AJ53" t="s" s="2">
         <v>359</v>
       </c>
-      <c r="AI53" t="s" s="2">
-        <v>365</v>
-      </c>
-      <c r="AJ53" t="s" s="2">
-        <v>361</v>
-      </c>
       <c r="AK53" t="s" s="2">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AM53" t="s" s="2">
         <v>45</v>
@@ -7677,7 +7668,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7703,10 +7694,10 @@
         <v>124</v>
       </c>
       <c r="K54" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="L54" t="s" s="2">
         <v>252</v>
-      </c>
-      <c r="L54" t="s" s="2">
-        <v>253</v>
       </c>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
@@ -7757,28 +7748,28 @@
         <v>45</v>
       </c>
       <c r="AE54" t="s" s="2">
+        <v>253</v>
+      </c>
+      <c r="AF54" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG54" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL54" t="s" s="2">
         <v>254</v>
-      </c>
-      <c r="AF54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG54" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL54" t="s" s="2">
-        <v>255</v>
       </c>
       <c r="AM54" t="s" s="2">
         <v>45</v>
@@ -7792,7 +7783,7 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -7821,7 +7812,7 @@
         <v>99</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="M55" t="s" s="2">
         <v>101</v>
@@ -7874,7 +7865,7 @@
         <v>45</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>43</v>
@@ -7895,7 +7886,7 @@
         <v>45</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AM55" t="s" s="2">
         <v>45</v>
@@ -7909,11 +7900,11 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" t="s" s="2">
@@ -7938,7 +7929,7 @@
         <v>104</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="M56" t="s" s="2">
         <v>101</v>
@@ -7991,7 +7982,7 @@
         <v>45</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>43</v>
@@ -8024,9 +8015,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="57" hidden="true">
+    <row r="57">
       <c r="A57" t="s" s="2">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -8040,7 +8031,7 @@
         <v>52</v>
       </c>
       <c r="G57" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H57" t="s" s="2">
         <v>45</v>
@@ -8049,16 +8040,16 @@
         <v>45</v>
       </c>
       <c r="J57" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="K57" t="s" s="2">
+        <v>370</v>
+      </c>
+      <c r="L57" t="s" s="2">
         <v>371</v>
       </c>
-      <c r="K57" t="s" s="2">
+      <c r="M57" t="s" s="2">
         <v>372</v>
-      </c>
-      <c r="L57" t="s" s="2">
-        <v>373</v>
-      </c>
-      <c r="M57" t="s" s="2">
-        <v>374</v>
       </c>
       <c r="N57" s="2"/>
       <c r="O57" t="s" s="2">
@@ -8084,13 +8075,13 @@
         <v>45</v>
       </c>
       <c r="W57" t="s" s="2">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="X57" t="s" s="2">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="Y57" t="s" s="2">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="Z57" t="s" s="2">
         <v>45</v>
@@ -8108,7 +8099,7 @@
         <v>45</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>52</v>
@@ -8123,13 +8114,13 @@
         <v>45</v>
       </c>
       <c r="AJ57" t="s" s="2">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AK57" t="s" s="2">
         <v>112</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AM57" t="s" s="2">
         <v>45</v>
@@ -8143,7 +8134,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -8166,19 +8157,19 @@
         <v>45</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="K58" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="L58" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="M58" t="s" s="2">
         <v>376</v>
       </c>
-      <c r="L58" t="s" s="2">
+      <c r="N58" t="s" s="2">
         <v>377</v>
-      </c>
-      <c r="M58" t="s" s="2">
-        <v>378</v>
-      </c>
-      <c r="N58" t="s" s="2">
-        <v>379</v>
       </c>
       <c r="O58" t="s" s="2">
         <v>45</v>
@@ -8203,13 +8194,13 @@
         <v>45</v>
       </c>
       <c r="W58" t="s" s="2">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="X58" t="s" s="2">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="Y58" t="s" s="2">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="Z58" t="s" s="2">
         <v>45</v>
@@ -8227,7 +8218,7 @@
         <v>45</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>43</v>
@@ -8236,19 +8227,19 @@
         <v>52</v>
       </c>
       <c r="AH58" t="s" s="2">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="AI58" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AJ58" t="s" s="2">
-        <v>381</v>
+        <v>45</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AM58" t="s" s="2">
         <v>45</v>
@@ -8260,9 +8251,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="59" hidden="true">
+    <row r="59">
       <c r="A59" t="s" s="2">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -8276,7 +8267,7 @@
         <v>44</v>
       </c>
       <c r="G59" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H59" t="s" s="2">
         <v>45</v>
@@ -8288,16 +8279,16 @@
         <v>45</v>
       </c>
       <c r="K59" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="L59" t="s" s="2">
+        <v>381</v>
+      </c>
+      <c r="M59" t="s" s="2">
+        <v>382</v>
+      </c>
+      <c r="N59" t="s" s="2">
         <v>383</v>
-      </c>
-      <c r="L59" t="s" s="2">
-        <v>384</v>
-      </c>
-      <c r="M59" t="s" s="2">
-        <v>385</v>
-      </c>
-      <c r="N59" t="s" s="2">
-        <v>386</v>
       </c>
       <c r="O59" t="s" s="2">
         <v>45</v>
@@ -8346,7 +8337,7 @@
         <v>45</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>43</v>
@@ -8355,19 +8346,19 @@
         <v>44</v>
       </c>
       <c r="AH59" t="s" s="2">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AI59" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="AM59" t="s" s="2">
         <v>45</v>

</xml_diff>

<commit_message>
edits and updates based on May30 call
</commit_message>
<xml_diff>
--- a/docs/q.xlsx
+++ b/docs/q.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$66</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2485" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2449" uniqueCount="405">
   <si>
     <t>Path</t>
   </si>
@@ -298,7 +298,7 @@
 anonymous resourcescontained resources</t>
   </si>
   <si>
-    <t xml:space="preserve">Resource {[]} {[]}
+    <t xml:space="preserve">ValueSet {[CanonicalType[http://fhir.org/guides/argonaut-questionnaire/StructureDefinition/qcvs]]} {[]}
 </t>
   </si>
   <si>
@@ -309,6 +309,9 @@
   </si>
   <si>
     <t>This should never be done when the content can be identified properly, as once identification is lost, it is extremely difficult (and context dependent) to restore it again.</t>
+  </si>
+  <si>
+    <t>The contained Valuesets are referenced when using the `.options` element.</t>
   </si>
   <si>
     <t>DomainResource.contained</t>
@@ -834,13 +837,6 @@
   </si>
   <si>
     <t>tl2</t>
-  </si>
-  <si>
-    <t>s1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension {[CanonicalType[http://fhir.org/guides/argonaut-questionnaire/StructureDefinition/extension-score]]} {[]}
-</t>
   </si>
   <si>
     <t>Questionnaire.item.modifierExtension</t>
@@ -998,6 +994,10 @@
     <t>s2</t>
   </si>
   <si>
+    <t xml:space="preserve">Extension {[CanonicalType[http://fhir.org/guides/argonaut-questionnaire/StructureDefinition/extension-score]]} {[]}
+</t>
+  </si>
+  <si>
     <t>Questionnaire.item.type.value</t>
   </si>
   <si>
@@ -1190,11 +1190,15 @@
     <t>A reference to a value set containing a list of codes representing permitted answers for a "choice" or "open-choice" question.</t>
   </si>
   <si>
-    <t>LOINC defines many useful value sets for questionnaire responses. See [LOINC Answer Lists](loinc.html#alist). The value may come from the ElementDefinition referred to by .definition.</t>
+    <t>When used, references the contained ValueSets.</t>
   </si>
   <si>
     <t>que-4
 que-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q-1:SHALL be a reference to a contained valueset. {reference.startsWith('#')}
+</t>
   </si>
   <si>
     <t>Questionnaire.group.question.options</t>
@@ -1438,7 +1442,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AP67"/>
+  <dimension ref="A1:AP66"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -2313,7 +2317,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" hidden="true">
+    <row r="8">
       <c r="A8" t="s" s="2">
         <v>88</v>
       </c>
@@ -2329,7 +2333,7 @@
         <v>44</v>
       </c>
       <c r="G8" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H8" t="s" s="2">
         <v>45</v>
@@ -2349,7 +2353,9 @@
       <c r="M8" t="s" s="2">
         <v>93</v>
       </c>
-      <c r="N8" s="2"/>
+      <c r="N8" t="s" s="2">
+        <v>94</v>
+      </c>
       <c r="O8" t="s" s="2">
         <v>45</v>
       </c>
@@ -2397,7 +2403,7 @@
         <v>45</v>
       </c>
       <c r="AE8" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AF8" t="s" s="2">
         <v>43</v>
@@ -2418,7 +2424,7 @@
         <v>45</v>
       </c>
       <c r="AL8" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AM8" t="s" s="2">
         <v>45</v>
@@ -2432,7 +2438,7 @@
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
@@ -2455,13 +2461,13 @@
         <v>45</v>
       </c>
       <c r="J9" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -2500,17 +2506,17 @@
         <v>45</v>
       </c>
       <c r="AA9" t="s" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AB9" s="2"/>
       <c r="AC9" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD9" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AF9" t="s" s="2">
         <v>43</v>
@@ -2545,10 +2551,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C10" t="s" s="2">
         <v>45</v>
@@ -2570,13 +2576,13 @@
         <v>45</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -2627,7 +2633,7 @@
         <v>45</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AF10" t="s" s="2">
         <v>43</v>
@@ -2662,11 +2668,11 @@
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" t="s" s="2">
@@ -2685,16 +2691,16 @@
         <v>45</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" t="s" s="2">
@@ -2744,7 +2750,7 @@
         <v>45</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>43</v>
@@ -2765,7 +2771,7 @@
         <v>45</v>
       </c>
       <c r="AL11" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AM11" t="s" s="2">
         <v>45</v>
@@ -2779,7 +2785,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
@@ -2805,16 +2811,16 @@
         <v>65</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="N12" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="O12" t="s" s="2">
         <v>45</v>
@@ -2863,7 +2869,7 @@
         <v>45</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>43</v>
@@ -2878,16 +2884,16 @@
         <v>45</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="AK12" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AL12" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="AM12" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AN12" t="s" s="2">
         <v>45</v>
@@ -2898,7 +2904,7 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -2921,19 +2927,19 @@
         <v>53</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="N13" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="O13" t="s" s="2">
         <v>45</v>
@@ -2982,7 +2988,7 @@
         <v>45</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>43</v>
@@ -3003,13 +3009,13 @@
         <v>45</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AM13" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AN13" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AO13" t="s" s="2">
         <v>45</v>
@@ -3017,7 +3023,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -3040,16 +3046,16 @@
         <v>53</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" t="s" s="2">
@@ -3099,7 +3105,7 @@
         <v>45</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>43</v>
@@ -3114,16 +3120,16 @@
         <v>45</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AL14" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AM14" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AN14" t="s" s="2">
         <v>45</v>
@@ -3134,7 +3140,7 @@
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -3157,19 +3163,19 @@
         <v>53</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="N15" t="s" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="O15" t="s" s="2">
         <v>45</v>
@@ -3218,7 +3224,7 @@
         <v>45</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>43</v>
@@ -3239,7 +3245,7 @@
         <v>45</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AM15" t="s" s="2">
         <v>45</v>
@@ -3253,7 +3259,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -3276,16 +3282,16 @@
         <v>53</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" t="s" s="2">
@@ -3335,7 +3341,7 @@
         <v>45</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>43</v>
@@ -3350,13 +3356,13 @@
         <v>45</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="AM16" t="s" s="2">
         <v>45</v>
@@ -3370,7 +3376,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -3396,13 +3402,13 @@
         <v>71</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" t="s" s="2">
@@ -3428,13 +3434,13 @@
         <v>45</v>
       </c>
       <c r="W17" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="X17" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="Y17" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="Z17" t="s" s="2">
         <v>45</v>
@@ -3452,7 +3458,7 @@
         <v>45</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>52</v>
@@ -3467,16 +3473,16 @@
         <v>45</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AN17" t="s" s="2">
         <v>45</v>
@@ -3487,7 +3493,7 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -3510,19 +3516,19 @@
         <v>53</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="N18" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="O18" t="s" s="2">
         <v>45</v>
@@ -3571,7 +3577,7 @@
         <v>45</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>43</v>
@@ -3592,10 +3598,10 @@
         <v>45</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="AN18" t="s" s="2">
         <v>45</v>
@@ -3606,11 +3612,11 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
@@ -3629,16 +3635,16 @@
         <v>53</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
@@ -3688,7 +3694,7 @@
         <v>45</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>43</v>
@@ -3709,10 +3715,10 @@
         <v>45</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="AN19" t="s" s="2">
         <v>45</v>
@@ -3723,7 +3729,7 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3746,19 +3752,19 @@
         <v>53</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="N20" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="O20" t="s" s="2">
         <v>45</v>
@@ -3807,7 +3813,7 @@
         <v>45</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>43</v>
@@ -3828,10 +3834,10 @@
         <v>45</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AN20" t="s" s="2">
         <v>45</v>
@@ -3842,7 +3848,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3865,16 +3871,16 @@
         <v>45</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" t="s" s="2">
@@ -3924,7 +3930,7 @@
         <v>45</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>43</v>
@@ -3939,13 +3945,13 @@
         <v>45</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="AM21" t="s" s="2">
         <v>45</v>
@@ -3959,7 +3965,7 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3982,16 +3988,16 @@
         <v>45</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" t="s" s="2">
@@ -4041,7 +4047,7 @@
         <v>45</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>43</v>
@@ -4062,13 +4068,13 @@
         <v>45</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AO22" t="s" s="2">
         <v>45</v>
@@ -4076,7 +4082,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -4099,16 +4105,16 @@
         <v>45</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
@@ -4158,7 +4164,7 @@
         <v>45</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>43</v>
@@ -4179,13 +4185,13 @@
         <v>45</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="AM23" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AO23" t="s" s="2">
         <v>45</v>
@@ -4193,7 +4199,7 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4216,19 +4222,19 @@
         <v>45</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>45</v>
@@ -4277,7 +4283,7 @@
         <v>45</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>43</v>
@@ -4298,13 +4304,13 @@
         <v>45</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="AM24" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AN24" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AO24" t="s" s="2">
         <v>45</v>
@@ -4312,7 +4318,7 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4335,19 +4341,19 @@
         <v>53</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>45</v>
@@ -4396,7 +4402,7 @@
         <v>45</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>43</v>
@@ -4417,13 +4423,13 @@
         <v>45</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AM25" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AN25" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AO25" t="s" s="2">
         <v>45</v>
@@ -4431,7 +4437,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4454,19 +4460,19 @@
         <v>53</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>45</v>
@@ -4515,7 +4521,7 @@
         <v>45</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>43</v>
@@ -4536,7 +4542,7 @@
         <v>45</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AM26" t="s" s="2">
         <v>45</v>
@@ -4550,7 +4556,7 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4573,16 +4579,16 @@
         <v>53</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
@@ -4611,10 +4617,10 @@
         <v>75</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="Y27" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="Z27" t="s" s="2">
         <v>45</v>
@@ -4632,7 +4638,7 @@
         <v>45</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>43</v>
@@ -4653,7 +4659,7 @@
         <v>45</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AM27" t="s" s="2">
         <v>45</v>
@@ -4667,7 +4673,7 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4690,16 +4696,16 @@
         <v>53</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
@@ -4749,7 +4755,7 @@
         <v>45</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>43</v>
@@ -4770,7 +4776,7 @@
         <v>45</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AM28" t="s" s="2">
         <v>45</v>
@@ -4784,11 +4790,11 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" t="s" s="2">
@@ -4807,17 +4813,17 @@
         <v>45</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="M29" s="2"/>
       <c r="N29" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="O29" t="s" s="2">
         <v>45</v>
@@ -4866,7 +4872,7 @@
         <v>45</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>43</v>
@@ -4887,13 +4893,13 @@
         <v>45</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AM29" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AN29" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AO29" t="s" s="2">
         <v>45</v>
@@ -4901,7 +4907,7 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4924,17 +4930,17 @@
         <v>53</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="M30" s="2"/>
       <c r="N30" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="O30" t="s" s="2">
         <v>45</v>
@@ -4959,13 +4965,13 @@
         <v>45</v>
       </c>
       <c r="W30" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="X30" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="Y30" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="Z30" t="s" s="2">
         <v>45</v>
@@ -4983,7 +4989,7 @@
         <v>45</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
@@ -5004,7 +5010,7 @@
         <v>45</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="AM30" t="s" s="2">
         <v>45</v>
@@ -5018,7 +5024,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5044,13 +5050,13 @@
         <v>71</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
@@ -5076,13 +5082,13 @@
         <v>45</v>
       </c>
       <c r="W31" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="X31" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="Y31" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="Z31" t="s" s="2">
         <v>45</v>
@@ -5100,7 +5106,7 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
@@ -5121,7 +5127,7 @@
         <v>45</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AM31" t="s" s="2">
         <v>45</v>
@@ -5135,7 +5141,7 @@
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5158,16 +5164,16 @@
         <v>45</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
@@ -5217,7 +5223,7 @@
         <v>45</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>43</v>
@@ -5226,19 +5232,19 @@
         <v>44</v>
       </c>
       <c r="AH32" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AI32" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AM32" t="s" s="2">
         <v>45</v>
@@ -5252,7 +5258,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5275,13 +5281,13 @@
         <v>45</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -5332,7 +5338,7 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
@@ -5353,7 +5359,7 @@
         <v>45</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AM33" t="s" s="2">
         <v>45</v>
@@ -5367,7 +5373,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5390,13 +5396,13 @@
         <v>45</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -5435,17 +5441,17 @@
         <v>45</v>
       </c>
       <c r="AA34" t="s" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AB34" s="2"/>
       <c r="AC34" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD34" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5480,10 +5486,10 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C35" t="s" s="2">
         <v>45</v>
@@ -5505,13 +5511,13 @@
         <v>45</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -5562,7 +5568,7 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -5595,42 +5601,42 @@
         <v>45</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>259</v>
-      </c>
-      <c r="B36" t="s" s="2">
-        <v>262</v>
-      </c>
+        <v>263</v>
+      </c>
+      <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
-        <v>45</v>
+        <v>264</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F36" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="G36" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H36" t="s" s="2">
         <v>53</v>
       </c>
-      <c r="H36" t="s" s="2">
-        <v>45</v>
-      </c>
       <c r="I36" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>263</v>
+        <v>98</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="M36" s="2"/>
+        <v>265</v>
+      </c>
+      <c r="M36" t="s" s="2">
+        <v>110</v>
+      </c>
       <c r="N36" s="2"/>
       <c r="O36" t="s" s="2">
         <v>45</v>
@@ -5679,7 +5685,7 @@
         <v>45</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>43</v>
@@ -5700,7 +5706,7 @@
         <v>45</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>45</v>
+        <v>96</v>
       </c>
       <c r="AM36" t="s" s="2">
         <v>45</v>
@@ -5712,43 +5718,45 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" hidden="true">
+    <row r="37">
       <c r="A37" t="s" s="2">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
-        <v>265</v>
+        <v>45</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="F37" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="G37" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H37" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="I37" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>97</v>
+        <v>129</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>107</v>
+        <v>268</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>109</v>
-      </c>
-      <c r="N37" s="2"/>
+        <v>270</v>
+      </c>
+      <c r="N37" t="s" s="2">
+        <v>271</v>
+      </c>
       <c r="O37" t="s" s="2">
         <v>45</v>
       </c>
@@ -5799,10 +5807,10 @@
         <v>267</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="AG37" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="AH37" t="s" s="2">
         <v>45</v>
@@ -5811,13 +5819,13 @@
         <v>45</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>45</v>
+        <v>267</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>45</v>
+        <v>272</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>95</v>
+        <v>273</v>
       </c>
       <c r="AM37" t="s" s="2">
         <v>45</v>
@@ -5829,9 +5837,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5839,13 +5847,13 @@
       </c>
       <c r="D38" s="2"/>
       <c r="E38" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F38" t="s" s="2">
         <v>52</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="H38" t="s" s="2">
         <v>45</v>
@@ -5854,19 +5862,19 @@
         <v>45</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>128</v>
+        <v>65</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>45</v>
@@ -5915,10 +5923,10 @@
         <v>45</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>52</v>
@@ -5930,13 +5938,13 @@
         <v>45</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>268</v>
+        <v>45</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>273</v>
+        <v>45</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="AM38" t="s" s="2">
         <v>45</v>
@@ -5948,9 +5956,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" hidden="true">
+    <row r="39">
       <c r="A39" t="s" s="2">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5961,31 +5969,31 @@
         <v>43</v>
       </c>
       <c r="F39" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="G39" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H39" t="s" s="2">
         <v>45</v>
       </c>
       <c r="I39" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>65</v>
+        <v>231</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>45</v>
@@ -6010,13 +6018,13 @@
         <v>45</v>
       </c>
       <c r="W39" t="s" s="2">
-        <v>45</v>
+        <v>235</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>45</v>
+        <v>236</v>
       </c>
       <c r="Y39" t="s" s="2">
-        <v>45</v>
+        <v>237</v>
       </c>
       <c r="Z39" t="s" s="2">
         <v>45</v>
@@ -6034,28 +6042,28 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG39" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="AH39" t="s" s="2">
-        <v>45</v>
+        <v>251</v>
       </c>
       <c r="AI39" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>45</v>
+        <v>280</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>45</v>
+        <v>285</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>280</v>
+        <v>238</v>
       </c>
       <c r="AM39" t="s" s="2">
         <v>45</v>
@@ -6069,18 +6077,18 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
-        <v>45</v>
+        <v>287</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F40" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="G40" t="s" s="2">
         <v>53</v>
@@ -6089,22 +6097,22 @@
         <v>45</v>
       </c>
       <c r="I40" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>230</v>
+        <v>129</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>45</v>
@@ -6129,13 +6137,13 @@
         <v>45</v>
       </c>
       <c r="W40" t="s" s="2">
-        <v>234</v>
+        <v>45</v>
       </c>
       <c r="X40" t="s" s="2">
-        <v>235</v>
+        <v>45</v>
       </c>
       <c r="Y40" t="s" s="2">
-        <v>236</v>
+        <v>45</v>
       </c>
       <c r="Z40" t="s" s="2">
         <v>45</v>
@@ -6153,28 +6161,28 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG40" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="AH40" t="s" s="2">
-        <v>250</v>
+        <v>45</v>
       </c>
       <c r="AI40" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>237</v>
+        <v>293</v>
       </c>
       <c r="AM40" t="s" s="2">
         <v>45</v>
@@ -6188,11 +6196,11 @@
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
-        <v>288</v>
+        <v>45</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" t="s" s="2">
@@ -6208,23 +6216,19 @@
         <v>45</v>
       </c>
       <c r="I41" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>290</v>
-      </c>
-      <c r="M41" t="s" s="2">
-        <v>291</v>
-      </c>
-      <c r="N41" t="s" s="2">
-        <v>292</v>
-      </c>
+        <v>296</v>
+      </c>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
         <v>45</v>
       </c>
@@ -6272,7 +6276,7 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
@@ -6287,13 +6291,13 @@
         <v>45</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>294</v>
+        <v>181</v>
       </c>
       <c r="AM41" t="s" s="2">
         <v>45</v>
@@ -6307,7 +6311,7 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6315,7 +6319,7 @@
       </c>
       <c r="D42" s="2"/>
       <c r="E42" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="F42" t="s" s="2">
         <v>52</v>
@@ -6327,19 +6331,23 @@
         <v>45</v>
       </c>
       <c r="I42" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>128</v>
+        <v>71</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>297</v>
-      </c>
-      <c r="M42" s="2"/>
-      <c r="N42" s="2"/>
+        <v>300</v>
+      </c>
+      <c r="M42" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="N42" t="s" s="2">
+        <v>302</v>
+      </c>
       <c r="O42" t="s" s="2">
         <v>45</v>
       </c>
@@ -6363,13 +6371,13 @@
         <v>45</v>
       </c>
       <c r="W42" t="s" s="2">
-        <v>45</v>
+        <v>149</v>
       </c>
       <c r="X42" t="s" s="2">
-        <v>45</v>
+        <v>303</v>
       </c>
       <c r="Y42" t="s" s="2">
-        <v>45</v>
+        <v>304</v>
       </c>
       <c r="Z42" t="s" s="2">
         <v>45</v>
@@ -6387,10 +6395,10 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>52</v>
@@ -6402,13 +6410,13 @@
         <v>45</v>
       </c>
       <c r="AJ42" t="s" s="2">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>180</v>
+        <v>306</v>
       </c>
       <c r="AM42" t="s" s="2">
         <v>45</v>
@@ -6420,9 +6428,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6430,13 +6438,13 @@
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F43" t="s" s="2">
         <v>52</v>
       </c>
       <c r="G43" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="H43" t="s" s="2">
         <v>45</v>
@@ -6445,20 +6453,16 @@
         <v>45</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>71</v>
+        <v>129</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>301</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>302</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>303</v>
-      </c>
+        <v>308</v>
+      </c>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
         <v>45</v>
       </c>
@@ -6482,13 +6486,13 @@
         <v>45</v>
       </c>
       <c r="W43" t="s" s="2">
-        <v>148</v>
+        <v>45</v>
       </c>
       <c r="X43" t="s" s="2">
-        <v>304</v>
+        <v>45</v>
       </c>
       <c r="Y43" t="s" s="2">
-        <v>305</v>
+        <v>45</v>
       </c>
       <c r="Z43" t="s" s="2">
         <v>45</v>
@@ -6506,10 +6510,10 @@
         <v>45</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>299</v>
+        <v>258</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>52</v>
@@ -6521,13 +6525,13 @@
         <v>45</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>299</v>
+        <v>45</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>306</v>
+        <v>45</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>307</v>
+        <v>45</v>
       </c>
       <c r="AM43" t="s" s="2">
         <v>45</v>
@@ -6541,7 +6545,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6552,7 +6556,7 @@
         <v>43</v>
       </c>
       <c r="F44" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="G44" t="s" s="2">
         <v>45</v>
@@ -6564,13 +6568,13 @@
         <v>45</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>128</v>
+        <v>98</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>255</v>
+        <v>99</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>309</v>
+        <v>100</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -6609,25 +6613,23 @@
         <v>45</v>
       </c>
       <c r="AA44" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB44" t="s" s="2">
-        <v>45</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="AB44" s="2"/>
       <c r="AC44" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD44" t="s" s="2">
-        <v>45</v>
+        <v>102</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG44" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="AH44" t="s" s="2">
         <v>45</v>
@@ -6654,11 +6656,13 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" hidden="true">
+    <row r="45">
       <c r="A45" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="B45" t="s" s="2">
         <v>310</v>
       </c>
-      <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
         <v>45</v>
       </c>
@@ -6667,10 +6671,10 @@
         <v>43</v>
       </c>
       <c r="F45" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="G45" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H45" t="s" s="2">
         <v>45</v>
@@ -6679,13 +6683,13 @@
         <v>45</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>97</v>
+        <v>311</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -6724,17 +6728,19 @@
         <v>45</v>
       </c>
       <c r="AA45" t="s" s="2">
-        <v>100</v>
-      </c>
-      <c r="AB45" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="AB45" t="s" s="2">
+        <v>45</v>
+      </c>
       <c r="AC45" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD45" t="s" s="2">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>43</v>
@@ -6767,13 +6773,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>310</v>
-      </c>
-      <c r="B46" t="s" s="2">
-        <v>311</v>
-      </c>
+        <v>312</v>
+      </c>
+      <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
         <v>45</v>
       </c>
@@ -6785,7 +6789,7 @@
         <v>52</v>
       </c>
       <c r="G46" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="H46" t="s" s="2">
         <v>45</v>
@@ -6794,13 +6798,13 @@
         <v>45</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>263</v>
+        <v>313</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>98</v>
+        <v>314</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>99</v>
+        <v>314</v>
       </c>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -6851,13 +6855,13 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>260</v>
+        <v>315</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG46" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="AH46" t="s" s="2">
         <v>45</v>
@@ -6886,7 +6890,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6897,28 +6901,32 @@
         <v>43</v>
       </c>
       <c r="F47" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="G47" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H47" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="I47" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>313</v>
+        <v>247</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>314</v>
-      </c>
-      <c r="M47" s="2"/>
-      <c r="N47" s="2"/>
+        <v>318</v>
+      </c>
+      <c r="M47" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="N47" t="s" s="2">
+        <v>320</v>
+      </c>
       <c r="O47" t="s" s="2">
         <v>45</v>
       </c>
@@ -6966,19 +6974,19 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG47" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="AH47" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI47" t="s" s="2">
-        <v>45</v>
+        <v>321</v>
       </c>
       <c r="AJ47" t="s" s="2">
         <v>45</v>
@@ -6987,7 +6995,7 @@
         <v>45</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>45</v>
+        <v>306</v>
       </c>
       <c r="AM47" t="s" s="2">
         <v>45</v>
@@ -7001,7 +7009,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -7012,32 +7020,28 @@
         <v>43</v>
       </c>
       <c r="F48" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="G48" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H48" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="I48" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>246</v>
+        <v>129</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>317</v>
+        <v>256</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>318</v>
-      </c>
-      <c r="M48" t="s" s="2">
-        <v>319</v>
-      </c>
-      <c r="N48" t="s" s="2">
-        <v>320</v>
-      </c>
+        <v>257</v>
+      </c>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
         <v>45</v>
       </c>
@@ -7085,19 +7089,19 @@
         <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>316</v>
+        <v>258</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG48" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="AH48" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>321</v>
+        <v>45</v>
       </c>
       <c r="AJ48" t="s" s="2">
         <v>45</v>
@@ -7106,7 +7110,7 @@
         <v>45</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>307</v>
+        <v>259</v>
       </c>
       <c r="AM48" t="s" s="2">
         <v>45</v>
@@ -7120,18 +7124,18 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
-        <v>45</v>
+        <v>107</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F49" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="G49" t="s" s="2">
         <v>45</v>
@@ -7143,15 +7147,17 @@
         <v>45</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>128</v>
+        <v>98</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>255</v>
+        <v>324</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>256</v>
-      </c>
-      <c r="M49" s="2"/>
+        <v>325</v>
+      </c>
+      <c r="M49" t="s" s="2">
+        <v>110</v>
+      </c>
       <c r="N49" s="2"/>
       <c r="O49" t="s" s="2">
         <v>45</v>
@@ -7200,13 +7206,13 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG49" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="AH49" t="s" s="2">
         <v>45</v>
@@ -7221,7 +7227,7 @@
         <v>45</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AM49" t="s" s="2">
         <v>45</v>
@@ -7235,11 +7241,11 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
-        <v>106</v>
+        <v>264</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
@@ -7252,22 +7258,22 @@
         <v>45</v>
       </c>
       <c r="H50" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="I50" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>324</v>
+        <v>108</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>325</v>
+        <v>265</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" t="s" s="2">
@@ -7317,7 +7323,7 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>43</v>
@@ -7338,7 +7344,7 @@
         <v>45</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>258</v>
+        <v>96</v>
       </c>
       <c r="AM50" t="s" s="2">
         <v>45</v>
@@ -7352,39 +7358,39 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
-        <v>265</v>
+        <v>45</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="F51" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="G51" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H51" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="I51" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>97</v>
+        <v>129</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>107</v>
+        <v>328</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>266</v>
+        <v>329</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>109</v>
+        <v>330</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" t="s" s="2">
@@ -7434,13 +7440,13 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>267</v>
+        <v>327</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="AG51" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="AH51" t="s" s="2">
         <v>45</v>
@@ -7455,7 +7461,7 @@
         <v>45</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>95</v>
+        <v>306</v>
       </c>
       <c r="AM51" t="s" s="2">
         <v>45</v>
@@ -7469,7 +7475,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7477,7 +7483,7 @@
       </c>
       <c r="D52" s="2"/>
       <c r="E52" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F52" t="s" s="2">
         <v>52</v>
@@ -7492,16 +7498,16 @@
         <v>45</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>128</v>
+        <v>155</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" t="s" s="2">
@@ -7551,16 +7557,16 @@
         <v>45</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>52</v>
       </c>
       <c r="AH52" t="s" s="2">
-        <v>45</v>
+        <v>335</v>
       </c>
       <c r="AI52" t="s" s="2">
         <v>45</v>
@@ -7572,7 +7578,7 @@
         <v>45</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AM52" t="s" s="2">
         <v>45</v>
@@ -7586,7 +7592,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7609,16 +7615,16 @@
         <v>45</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>154</v>
+        <v>337</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>332</v>
+        <v>338</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="N53" s="2"/>
       <c r="O53" t="s" s="2">
@@ -7644,13 +7650,13 @@
         <v>45</v>
       </c>
       <c r="W53" t="s" s="2">
-        <v>45</v>
+        <v>235</v>
       </c>
       <c r="X53" t="s" s="2">
-        <v>45</v>
+        <v>341</v>
       </c>
       <c r="Y53" t="s" s="2">
-        <v>45</v>
+        <v>342</v>
       </c>
       <c r="Z53" t="s" s="2">
         <v>45</v>
@@ -7668,7 +7674,7 @@
         <v>45</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>43</v>
@@ -7689,7 +7695,7 @@
         <v>45</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AM53" t="s" s="2">
         <v>45</v>
@@ -7701,9 +7707,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="54" hidden="true">
+    <row r="54">
       <c r="A54" t="s" s="2">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7717,7 +7723,7 @@
         <v>52</v>
       </c>
       <c r="G54" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H54" t="s" s="2">
         <v>45</v>
@@ -7726,20 +7732,20 @@
         <v>45</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>337</v>
+        <v>155</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>338</v>
+        <v>344</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="N54" s="2"/>
       <c r="O54" t="s" s="2">
-        <v>45</v>
+        <v>347</v>
       </c>
       <c r="P54" s="2"/>
       <c r="Q54" t="s" s="2">
@@ -7761,13 +7767,13 @@
         <v>45</v>
       </c>
       <c r="W54" t="s" s="2">
-        <v>234</v>
+        <v>45</v>
       </c>
       <c r="X54" t="s" s="2">
-        <v>341</v>
+        <v>45</v>
       </c>
       <c r="Y54" t="s" s="2">
-        <v>342</v>
+        <v>45</v>
       </c>
       <c r="Z54" t="s" s="2">
         <v>45</v>
@@ -7785,7 +7791,7 @@
         <v>45</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>43</v>
@@ -7794,19 +7800,19 @@
         <v>52</v>
       </c>
       <c r="AH54" t="s" s="2">
-        <v>335</v>
+        <v>348</v>
       </c>
       <c r="AI54" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AJ54" t="s" s="2">
-        <v>45</v>
+        <v>343</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>45</v>
+        <v>349</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AM54" t="s" s="2">
         <v>45</v>
@@ -7820,7 +7826,7 @@
     </row>
     <row r="55">
       <c r="A55" t="s" s="2">
-        <v>343</v>
+        <v>350</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -7843,18 +7849,20 @@
         <v>45</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>344</v>
+        <v>351</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>345</v>
+        <v>352</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>346</v>
-      </c>
-      <c r="N55" s="2"/>
+        <v>353</v>
+      </c>
+      <c r="N55" t="s" s="2">
+        <v>354</v>
+      </c>
       <c r="O55" t="s" s="2">
         <v>347</v>
       </c>
@@ -7902,7 +7910,7 @@
         <v>45</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>343</v>
+        <v>350</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>43</v>
@@ -7917,13 +7925,13 @@
         <v>45</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>343</v>
+        <v>350</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AM55" t="s" s="2">
         <v>45</v>
@@ -7935,9 +7943,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7951,7 +7959,7 @@
         <v>52</v>
       </c>
       <c r="G56" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="H56" t="s" s="2">
         <v>45</v>
@@ -7960,22 +7968,22 @@
         <v>45</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="N56" t="s" s="2">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="O56" t="s" s="2">
-        <v>347</v>
+        <v>45</v>
       </c>
       <c r="P56" s="2"/>
       <c r="Q56" t="s" s="2">
@@ -8021,7 +8029,7 @@
         <v>45</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>43</v>
@@ -8030,19 +8038,19 @@
         <v>52</v>
       </c>
       <c r="AH56" t="s" s="2">
-        <v>348</v>
+        <v>361</v>
       </c>
       <c r="AI56" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AJ56" t="s" s="2">
-        <v>350</v>
+        <v>45</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>355</v>
+        <v>45</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AM56" t="s" s="2">
         <v>45</v>
@@ -8056,7 +8064,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -8079,20 +8087,18 @@
         <v>45</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>154</v>
+        <v>363</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>357</v>
+        <v>364</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>359</v>
-      </c>
-      <c r="N57" t="s" s="2">
-        <v>360</v>
-      </c>
+        <v>366</v>
+      </c>
+      <c r="N57" s="2"/>
       <c r="O57" t="s" s="2">
         <v>45</v>
       </c>
@@ -8140,7 +8146,7 @@
         <v>45</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>43</v>
@@ -8149,7 +8155,7 @@
         <v>52</v>
       </c>
       <c r="AH57" t="s" s="2">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="AI57" t="s" s="2">
         <v>45</v>
@@ -8161,7 +8167,7 @@
         <v>45</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AM57" t="s" s="2">
         <v>45</v>
@@ -8170,12 +8176,12 @@
         <v>45</v>
       </c>
       <c r="AO57" t="s" s="2">
-        <v>45</v>
+        <v>96</v>
       </c>
     </row>
-    <row r="58" hidden="true">
+    <row r="58">
       <c r="A58" t="s" s="2">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -8189,7 +8195,7 @@
         <v>52</v>
       </c>
       <c r="G58" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H58" t="s" s="2">
         <v>45</v>
@@ -8198,16 +8204,16 @@
         <v>45</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="N58" s="2"/>
       <c r="O58" t="s" s="2">
@@ -8257,7 +8263,7 @@
         <v>45</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>43</v>
@@ -8266,19 +8272,19 @@
         <v>52</v>
       </c>
       <c r="AH58" t="s" s="2">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="AI58" t="s" s="2">
-        <v>45</v>
+        <v>374</v>
       </c>
       <c r="AJ58" t="s" s="2">
-        <v>45</v>
+        <v>368</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>45</v>
+        <v>375</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AM58" t="s" s="2">
         <v>45</v>
@@ -8287,12 +8293,12 @@
         <v>45</v>
       </c>
       <c r="AO58" t="s" s="2">
-        <v>95</v>
+        <v>45</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="2">
-        <v>368</v>
+        <v>376</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -8303,7 +8309,7 @@
         <v>43</v>
       </c>
       <c r="F59" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="G59" t="s" s="2">
         <v>53</v>
@@ -8315,16 +8321,16 @@
         <v>45</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>369</v>
+        <v>247</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>370</v>
+        <v>377</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>371</v>
+        <v>378</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="N59" s="2"/>
       <c r="O59" t="s" s="2">
@@ -8374,28 +8380,28 @@
         <v>45</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>368</v>
+        <v>376</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG59" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="AH59" t="s" s="2">
         <v>373</v>
       </c>
       <c r="AI59" t="s" s="2">
-        <v>45</v>
+        <v>380</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>368</v>
+        <v>376</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>374</v>
+        <v>381</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AM59" t="s" s="2">
         <v>45</v>
@@ -8407,9 +8413,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>375</v>
+        <v>382</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -8420,10 +8426,10 @@
         <v>43</v>
       </c>
       <c r="F60" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="G60" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="H60" t="s" s="2">
         <v>45</v>
@@ -8432,17 +8438,15 @@
         <v>45</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>246</v>
+        <v>129</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>376</v>
+        <v>256</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>377</v>
-      </c>
-      <c r="M60" t="s" s="2">
-        <v>378</v>
-      </c>
+        <v>257</v>
+      </c>
+      <c r="M60" s="2"/>
       <c r="N60" s="2"/>
       <c r="O60" t="s" s="2">
         <v>45</v>
@@ -8491,28 +8495,28 @@
         <v>45</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>375</v>
+        <v>258</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG60" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="AH60" t="s" s="2">
-        <v>373</v>
+        <v>45</v>
       </c>
       <c r="AI60" t="s" s="2">
-        <v>379</v>
+        <v>45</v>
       </c>
       <c r="AJ60" t="s" s="2">
-        <v>375</v>
+        <v>45</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>380</v>
+        <v>45</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>307</v>
+        <v>259</v>
       </c>
       <c r="AM60" t="s" s="2">
         <v>45</v>
@@ -8526,7 +8530,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8537,7 +8541,7 @@
         <v>43</v>
       </c>
       <c r="F61" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="G61" t="s" s="2">
         <v>45</v>
@@ -8549,13 +8553,13 @@
         <v>45</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>128</v>
+        <v>98</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>255</v>
+        <v>99</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>256</v>
+        <v>100</v>
       </c>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
@@ -8594,25 +8598,23 @@
         <v>45</v>
       </c>
       <c r="AA61" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB61" t="s" s="2">
-        <v>45</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="AB61" s="2"/>
       <c r="AC61" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD61" t="s" s="2">
-        <v>45</v>
+        <v>102</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG61" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="AH61" t="s" s="2">
         <v>45</v>
@@ -8627,7 +8629,7 @@
         <v>45</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>258</v>
+        <v>45</v>
       </c>
       <c r="AM61" t="s" s="2">
         <v>45</v>
@@ -8639,11 +8641,13 @@
         <v>45</v>
       </c>
     </row>
-    <row r="62" hidden="true">
+    <row r="62">
       <c r="A62" t="s" s="2">
-        <v>382</v>
-      </c>
-      <c r="B62" s="2"/>
+        <v>383</v>
+      </c>
+      <c r="B62" t="s" s="2">
+        <v>384</v>
+      </c>
       <c r="C62" t="s" s="2">
         <v>45</v>
       </c>
@@ -8652,10 +8656,10 @@
         <v>43</v>
       </c>
       <c r="F62" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="G62" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H62" t="s" s="2">
         <v>45</v>
@@ -8664,13 +8668,13 @@
         <v>45</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>97</v>
+        <v>311</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
@@ -8709,17 +8713,19 @@
         <v>45</v>
       </c>
       <c r="AA62" t="s" s="2">
-        <v>100</v>
-      </c>
-      <c r="AB62" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="AB62" t="s" s="2">
+        <v>45</v>
+      </c>
       <c r="AC62" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD62" t="s" s="2">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>43</v>
@@ -8752,42 +8758,42 @@
         <v>45</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>382</v>
-      </c>
-      <c r="B63" t="s" s="2">
-        <v>383</v>
-      </c>
+        <v>385</v>
+      </c>
+      <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
-        <v>45</v>
+        <v>264</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F63" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="G63" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H63" t="s" s="2">
         <v>53</v>
       </c>
-      <c r="H63" t="s" s="2">
-        <v>45</v>
-      </c>
       <c r="I63" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="J63" t="s" s="2">
-        <v>263</v>
+        <v>98</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="M63" s="2"/>
+        <v>265</v>
+      </c>
+      <c r="M63" t="s" s="2">
+        <v>110</v>
+      </c>
       <c r="N63" s="2"/>
       <c r="O63" t="s" s="2">
         <v>45</v>
@@ -8836,7 +8842,7 @@
         <v>45</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>43</v>
@@ -8857,7 +8863,7 @@
         <v>45</v>
       </c>
       <c r="AL63" t="s" s="2">
-        <v>45</v>
+        <v>96</v>
       </c>
       <c r="AM63" t="s" s="2">
         <v>45</v>
@@ -8869,41 +8875,41 @@
         <v>45</v>
       </c>
     </row>
-    <row r="64" hidden="true">
+    <row r="64">
       <c r="A64" t="s" s="2">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
-        <v>265</v>
+        <v>45</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="F64" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="G64" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H64" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="I64" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>97</v>
+        <v>387</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>107</v>
+        <v>388</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>266</v>
+        <v>389</v>
       </c>
       <c r="M64" t="s" s="2">
-        <v>109</v>
+        <v>390</v>
       </c>
       <c r="N64" s="2"/>
       <c r="O64" t="s" s="2">
@@ -8929,13 +8935,13 @@
         <v>45</v>
       </c>
       <c r="W64" t="s" s="2">
-        <v>45</v>
+        <v>235</v>
       </c>
       <c r="X64" t="s" s="2">
-        <v>45</v>
+        <v>341</v>
       </c>
       <c r="Y64" t="s" s="2">
-        <v>45</v>
+        <v>342</v>
       </c>
       <c r="Z64" t="s" s="2">
         <v>45</v>
@@ -8953,13 +8959,13 @@
         <v>45</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>267</v>
+        <v>386</v>
       </c>
       <c r="AF64" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="AG64" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="AH64" t="s" s="2">
         <v>45</v>
@@ -8968,13 +8974,13 @@
         <v>45</v>
       </c>
       <c r="AJ64" t="s" s="2">
-        <v>45</v>
+        <v>386</v>
       </c>
       <c r="AK64" t="s" s="2">
-        <v>45</v>
+        <v>117</v>
       </c>
       <c r="AL64" t="s" s="2">
-        <v>95</v>
+        <v>306</v>
       </c>
       <c r="AM64" t="s" s="2">
         <v>45</v>
@@ -8986,9 +8992,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -8996,13 +9002,13 @@
       </c>
       <c r="D65" s="2"/>
       <c r="E65" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F65" t="s" s="2">
         <v>52</v>
       </c>
       <c r="G65" t="s" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="H65" t="s" s="2">
         <v>45</v>
@@ -9011,18 +9017,20 @@
         <v>45</v>
       </c>
       <c r="J65" t="s" s="2">
-        <v>386</v>
+        <v>337</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>387</v>
+        <v>392</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>388</v>
+        <v>393</v>
       </c>
       <c r="M65" t="s" s="2">
-        <v>389</v>
-      </c>
-      <c r="N65" s="2"/>
+        <v>394</v>
+      </c>
+      <c r="N65" t="s" s="2">
+        <v>395</v>
+      </c>
       <c r="O65" t="s" s="2">
         <v>45</v>
       </c>
@@ -9046,7 +9054,7 @@
         <v>45</v>
       </c>
       <c r="W65" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="X65" t="s" s="2">
         <v>341</v>
@@ -9070,28 +9078,28 @@
         <v>45</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="AF65" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="AG65" t="s" s="2">
         <v>52</v>
       </c>
       <c r="AH65" t="s" s="2">
-        <v>45</v>
+        <v>396</v>
       </c>
       <c r="AI65" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AJ65" t="s" s="2">
-        <v>385</v>
+        <v>45</v>
       </c>
       <c r="AK65" t="s" s="2">
-        <v>116</v>
+        <v>45</v>
       </c>
       <c r="AL65" t="s" s="2">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AM65" t="s" s="2">
         <v>45</v>
@@ -9103,9 +9111,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="66" hidden="true">
+    <row r="66">
       <c r="A66" t="s" s="2">
-        <v>390</v>
+        <v>397</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -9116,10 +9124,10 @@
         <v>43</v>
       </c>
       <c r="F66" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="G66" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H66" t="s" s="2">
         <v>45</v>
@@ -9128,19 +9136,19 @@
         <v>45</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>337</v>
+        <v>45</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>391</v>
+        <v>398</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>392</v>
+        <v>399</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>393</v>
+        <v>400</v>
       </c>
       <c r="N66" t="s" s="2">
-        <v>394</v>
+        <v>401</v>
       </c>
       <c r="O66" t="s" s="2">
         <v>45</v>
@@ -9165,13 +9173,13 @@
         <v>45</v>
       </c>
       <c r="W66" t="s" s="2">
-        <v>234</v>
+        <v>45</v>
       </c>
       <c r="X66" t="s" s="2">
-        <v>341</v>
+        <v>45</v>
       </c>
       <c r="Y66" t="s" s="2">
-        <v>342</v>
+        <v>45</v>
       </c>
       <c r="Z66" t="s" s="2">
         <v>45</v>
@@ -9189,28 +9197,28 @@
         <v>45</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>390</v>
+        <v>397</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG66" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="AH66" t="s" s="2">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="AI66" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AJ66" t="s" s="2">
-        <v>45</v>
+        <v>397</v>
       </c>
       <c r="AK66" t="s" s="2">
-        <v>45</v>
+        <v>403</v>
       </c>
       <c r="AL66" t="s" s="2">
-        <v>307</v>
+        <v>404</v>
       </c>
       <c r="AM66" t="s" s="2">
         <v>45</v>
@@ -9219,130 +9227,11 @@
         <v>45</v>
       </c>
       <c r="AO66" t="s" s="2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="s" s="2">
-        <v>396</v>
-      </c>
-      <c r="B67" s="2"/>
-      <c r="C67" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="D67" s="2"/>
-      <c r="E67" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="F67" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="G67" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="H67" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="I67" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="J67" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="K67" t="s" s="2">
-        <v>397</v>
-      </c>
-      <c r="L67" t="s" s="2">
-        <v>398</v>
-      </c>
-      <c r="M67" t="s" s="2">
-        <v>399</v>
-      </c>
-      <c r="N67" t="s" s="2">
-        <v>400</v>
-      </c>
-      <c r="O67" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="P67" s="2"/>
-      <c r="Q67" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="R67" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="S67" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="T67" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="U67" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="V67" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="W67" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="X67" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Y67" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Z67" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA67" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB67" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC67" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD67" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE67" t="s" s="2">
-        <v>396</v>
-      </c>
-      <c r="AF67" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG67" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH67" t="s" s="2">
-        <v>401</v>
-      </c>
-      <c r="AI67" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ67" t="s" s="2">
-        <v>396</v>
-      </c>
-      <c r="AK67" t="s" s="2">
-        <v>402</v>
-      </c>
-      <c r="AL67" t="s" s="2">
-        <v>403</v>
-      </c>
-      <c r="AM67" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AN67" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO67" t="s" s="2">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO67">
+  <autoFilter ref="A1:AO66">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -9352,7 +9241,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI66">
+  <conditionalFormatting sqref="A2:AI65">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
add adaptive wf draft
</commit_message>
<xml_diff>
--- a/docs/q.xlsx
+++ b/docs/q.xlsx
@@ -3727,7 +3727,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" hidden="true">
+    <row r="20">
       <c r="A20" t="s" s="2">
         <v>169</v>
       </c>
@@ -3743,7 +3743,7 @@
         <v>52</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H20" t="s" s="2">
         <v>45</v>
@@ -3828,10 +3828,10 @@
         <v>45</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>45</v>
+        <v>169</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>45</v>
+        <v>169</v>
       </c>
       <c r="AL20" t="s" s="2">
         <v>174</v>

</xml_diff>